<commit_message>
powerpoint 50% & update productbacklog
</commit_message>
<xml_diff>
--- a/Documenten/productbacklog.xlsx
+++ b/Documenten/productbacklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrnl-my.sharepoint.com/personal/0987057_hr_nl/Documents/2021 Technische informatica 2/Project-5-6/Documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="8_{C8EFED4C-861F-4D9A-A52C-382DCF3D3507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B68E3C36-4C2F-4989-BFF5-44FCBC11E5F1}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="8_{C8EFED4C-861F-4D9A-A52C-382DCF3D3507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{50A71402-4DA1-41EE-822E-D438FF356651}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="16080" windowWidth="29040" windowHeight="16440" xr2:uid="{AB4C6EDC-C71E-401F-AB46-2C9C4233DE0F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -84,9 +84,6 @@
     <t>De berichten zijn volgens het NMEA protocol, Maximale latency 20ms van het eene component naar het ander component. Dit netwerk moet robuust zijn:{stevig, spatwater overleg PO concreete eisen}</t>
   </si>
   <si>
-    <t>Wat zijn de eisen voor de robuustheid, later bespreken</t>
-  </si>
-  <si>
     <t>3a</t>
   </si>
   <si>
@@ -193,13 +190,19 @@
   </si>
   <si>
     <t>Alle functies en data leveranciers/vragen zijn te vinden in de decompositie, alle vertakkingen zijn uitgewerkt zodat er duidelijk wordt waar verstoringen zitten en wat de verschillende eisen van componenten zijn</t>
+  </si>
+  <si>
+    <t>Wat zijn de eisen voor de robuustheid, later bespreken, experimenteel onderzoek</t>
+  </si>
+  <si>
+    <t>Literatuur onderzoek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,12 +276,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
@@ -286,6 +283,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,8 +306,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -335,22 +338,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -359,17 +359,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="5" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent6" xfId="5" builtinId="51"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -385,7 +388,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,11 +686,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279F508F-C923-4D8C-A0DD-EFAC01E2C0D1}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
@@ -698,7 +701,7 @@
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -721,14 +724,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A2" s="13">
+    <row r="2" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -742,253 +745,251 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="75">
-      <c r="A3" s="16">
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="45">
-      <c r="A5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="45">
-      <c r="A6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="60">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="45">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="90">
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="E9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="60">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="60">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="12"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="12"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -996,51 +997,51 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="12"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="12"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="12"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>21</v>
       </c>
@@ -1051,7 +1052,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -1062,7 +1063,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>23</v>
       </c>
@@ -1073,7 +1074,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1084,7 +1085,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1095,7 +1096,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1106,7 +1107,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1117,7 +1118,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1128,7 +1129,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1139,7 +1140,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1150,7 +1151,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1161,7 +1162,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1172,7 +1173,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1183,7 +1184,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1191,7 +1192,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1199,7 +1200,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1207,7 +1208,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1215,7 +1216,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1223,7 +1224,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1231,7 +1232,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1239,7 +1240,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>

</xml_diff>